<commit_message>
For Each Row in Data Table
</commit_message>
<xml_diff>
--- a/Data/Output/네이버증권.xlsx
+++ b/Data/Output/네이버증권.xlsx
@@ -7,6 +7,7 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="코스피원본_25-04-03" sheetId="2" r:id="rId2"/>
+    <x:sheet name="코스피원본_25-04-04" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -947,6 +948,586 @@
   </x:si>
   <x:si>
     <x:t>0.00%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+1.30%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+5.49%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 225</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-1.48%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 100</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+1.53%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-0.60%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 210</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+10.42%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+0.77%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+3.61%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+4.81%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-1.75%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+6.85%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 800</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-1.39%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 105</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+3.52%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 445</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+11.50%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알루코</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+3.88%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>삼성 레버리지 WTI원유 선물 ETN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 149</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-10.16%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+0.53%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 280</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-0.83%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 90</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-6.74%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 104</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 750</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-3.73%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 8,800</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-4.52%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+9.18%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 695</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-3.76%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-0.43%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>신한 레버리지 WTI원유 선물 ETN(H)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 86</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-9.07%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KODEX 미국달러선물인버스2X</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 165</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 330</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+4.26%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+0.65%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 85</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+2.91%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+3.17%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 130</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+3.78%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+0.87%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 255</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-0.76%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 183</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+11.35%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 450</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+1.91%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-0.64%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 550</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-4.27%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 680</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-3.67%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 350</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+2.65%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>N2 인버스 레버리지 WTI원유 선물 ETN(H)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+5.97%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 1,175</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-7.31%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 240</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+2.23%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+1.49%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+0.21%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-1.98%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 145</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+1.99%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KODEX 미국AI전력핵심인프라</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 720</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-6.81%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-0.36%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 300</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-0.23%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TIGER Fn반도체TOP10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-2.31%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 700</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+2.07%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+1.87%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>한국전력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 650</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+3.02%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>YG PLUS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 90</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+1.76%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-4.31%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TIGER 미국배당다우존스타겟커버드콜2호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 390</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-3.63%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-0.21%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-3.34%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>인디에프</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+5.75%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 505</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-2.42%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KODEX WTI원유선물인버스(H)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+3.85%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-0.32%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>한투 인버스 2X 코스닥150선물 ETN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 100</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 125</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KODEX 미국나스닥100(H)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 315</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-2.13%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 115</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-3.77%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RISE 미국S&amp;P500</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 670</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-3.82%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 770</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-3.79%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PLUS K방산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+0.52%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>한화솔루션</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 520</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+2.61%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>삼성 인버스 2X 은 선물 ETN(H)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+8.22%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KODEX 2차전지핵심소재10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 125</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 345</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-4.18%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+0.72%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 200</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+1.65%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KODEX 미국배당다우존스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-4.33%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 880</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-4.20%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+2.09%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TIGER 미국배당다우존스타겟데일리커버드콜</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-3.99%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상승
+ 17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+1.54%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 200</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TIGER 조선TOP10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-0.20%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>하락
+ 405</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-5.63%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+0.90%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ACE 포스코그룹포커스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+1.74%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KODEX 미국나스닥100데일리커버드콜OTM</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -3330,4 +3911,2044 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F162"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C3" s="0">
+        <x:v>2340</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>283</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="F3" s="0">
+        <x:v>64659270</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C4" s="0">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="F4" s="0">
+        <x:v>26144056</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C5" s="0">
+        <x:v>14940</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="F5" s="0">
+        <x:v>12013794</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C6" s="0">
+        <x:v>6645</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>289</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="F6" s="0">
+        <x:v>11774424</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="0">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C7" s="0">
+        <x:v>4110</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="F7" s="0">
+        <x:v>11696744</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C11" s="0">
+        <x:v>2225</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>294</x:v>
+      </x:c>
+      <x:c r="F11" s="0">
+        <x:v>10900825</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="A12" s="0">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C12" s="0">
+        <x:v>4600</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="F12" s="0">
+        <x:v>9282034</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="C13" s="0">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>298</x:v>
+      </x:c>
+      <x:c r="F13" s="0">
+        <x:v>8202243</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" s="0">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C14" s="0">
+        <x:v>937</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>299</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="F14" s="0">
+        <x:v>6309732</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="A15" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C15" s="0">
+        <x:v>899</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
+      <x:c r="F15" s="0">
+        <x:v>6046181</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" s="0">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C19" s="0">
+        <x:v>1104</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>303</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="F19" s="0">
+        <x:v>5104538</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="A20" s="0">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="C20" s="0">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="F20" s="0">
+        <x:v>4911478</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="A21" s="0">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C21" s="0">
+        <x:v>56800</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>306</x:v>
+      </x:c>
+      <x:c r="F21" s="0">
+        <x:v>4359977</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" s="0">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="C22" s="0">
+        <x:v>3085</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>307</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+      <x:c r="F22" s="0">
+        <x:v>2989775</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" s="0">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="C23" s="0">
+        <x:v>4315</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>310</x:v>
+      </x:c>
+      <x:c r="F23" s="0">
+        <x:v>2829980</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" s="0">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="C27" s="0">
+        <x:v>2140</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>312</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="F27" s="0">
+        <x:v>2715632</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" s="0">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>314</x:v>
+      </x:c>
+      <x:c r="C28" s="0">
+        <x:v>1318</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>315</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>316</x:v>
+      </x:c>
+      <x:c r="F28" s="0">
+        <x:v>2622558</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="A29" s="0">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C29" s="0">
+        <x:v>11385</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>317</x:v>
+      </x:c>
+      <x:c r="F29" s="0">
+        <x:v>2392932</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="A30" s="0">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C30" s="0">
+        <x:v>33475</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>318</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>319</x:v>
+      </x:c>
+      <x:c r="F30" s="0">
+        <x:v>2349086</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="A31" s="0">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C31" s="0">
+        <x:v>1245</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="F31" s="0">
+        <x:v>2338756</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" s="0">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C35" s="0">
+        <x:v>1997</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>322</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="F35" s="0">
+        <x:v>2193505</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" s="0">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C36" s="0">
+        <x:v>19365</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>323</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="F36" s="0">
+        <x:v>1773932</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="A37" s="0">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="C37" s="0">
+        <x:v>185800</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>325</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="F37" s="0">
+        <x:v>1756874</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="A38" s="0">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C38" s="0">
+        <x:v>1189</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>289</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>327</x:v>
+      </x:c>
+      <x:c r="F38" s="0">
+        <x:v>1719607</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="A39" s="0">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C39" s="0">
+        <x:v>17805</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>328</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="s">
+        <x:v>329</x:v>
+      </x:c>
+      <x:c r="F39" s="0">
+        <x:v>1654650</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:6">
+      <x:c r="A43" s="0">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C43" s="0">
+        <x:v>13950</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>330</x:v>
+      </x:c>
+      <x:c r="E43" s="0" t="s">
+        <x:v>331</x:v>
+      </x:c>
+      <x:c r="F43" s="0">
+        <x:v>1541878</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:6">
+      <x:c r="A44" s="0">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>332</x:v>
+      </x:c>
+      <x:c r="C44" s="0">
+        <x:v>862</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>333</x:v>
+      </x:c>
+      <x:c r="E44" s="0" t="s">
+        <x:v>334</x:v>
+      </x:c>
+      <x:c r="F44" s="0">
+        <x:v>1433060</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:6">
+      <x:c r="A45" s="0">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>335</x:v>
+      </x:c>
+      <x:c r="C45" s="0">
+        <x:v>5240</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>336</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="F45" s="0">
+        <x:v>1430517</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:6">
+      <x:c r="A46" s="0">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C46" s="0">
+        <x:v>576</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="E46" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="F46" s="0">
+        <x:v>1417101</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:6">
+      <x:c r="A47" s="0">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="C47" s="0">
+        <x:v>8080</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="F47" s="0">
+        <x:v>1407387</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:6">
+      <x:c r="A51" s="0">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="C51" s="0">
+        <x:v>7700</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>339</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="s">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="F51" s="0">
+        <x:v>1402898</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:6">
+      <x:c r="A52" s="0">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C52" s="0">
+        <x:v>7350</x:v>
+      </x:c>
+      <x:c r="D52" s="0" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="E52" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F52" s="0">
+        <x:v>1339736</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:6">
+      <x:c r="A53" s="0">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="C53" s="0">
+        <x:v>2120</x:v>
+      </x:c>
+      <x:c r="D53" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E53" s="0" t="s">
+        <x:v>342</x:v>
+      </x:c>
+      <x:c r="F53" s="0">
+        <x:v>1335817</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:6">
+      <x:c r="A54" s="0">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="C54" s="0">
+        <x:v>1010</x:v>
+      </x:c>
+      <x:c r="D54" s="0" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="E54" s="0" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="F54" s="0">
+        <x:v>1325352</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:6">
+      <x:c r="A55" s="0">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C55" s="0">
+        <x:v>1400</x:v>
+      </x:c>
+      <x:c r="D55" s="0" t="s">
+        <x:v>345</x:v>
+      </x:c>
+      <x:c r="E55" s="0" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="F55" s="0">
+        <x:v>1248757</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:6">
+      <x:c r="A59" s="0">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="C59" s="0">
+        <x:v>3565</x:v>
+      </x:c>
+      <x:c r="D59" s="0" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="E59" s="0" t="s">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="F59" s="0">
+        <x:v>1240231</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:6">
+      <x:c r="A60" s="0">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C60" s="0">
+        <x:v>2475</x:v>
+      </x:c>
+      <x:c r="D60" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E60" s="0" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="F60" s="0">
+        <x:v>1238586</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:6">
+      <x:c r="A61" s="0">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="C61" s="0">
+        <x:v>2895</x:v>
+      </x:c>
+      <x:c r="D61" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E61" s="0" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="F61" s="0">
+        <x:v>1168359</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:6">
+      <x:c r="A62" s="0">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="C62" s="0">
+        <x:v>33425</x:v>
+      </x:c>
+      <x:c r="D62" s="0" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="E62" s="0" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="F62" s="0">
+        <x:v>1133690</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:6">
+      <x:c r="A63" s="0">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="C63" s="0">
+        <x:v>1795</x:v>
+      </x:c>
+      <x:c r="D63" s="0" t="s">
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="E63" s="0" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="F63" s="0">
+        <x:v>1089997</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:6">
+      <x:c r="A67" s="0">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="C67" s="0">
+        <x:v>24050</x:v>
+      </x:c>
+      <x:c r="D67" s="0" t="s">
+        <x:v>353</x:v>
+      </x:c>
+      <x:c r="E67" s="0" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="F67" s="0">
+        <x:v>1064186</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:6">
+      <x:c r="A68" s="0">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="C68" s="0">
+        <x:v>9370</x:v>
+      </x:c>
+      <x:c r="D68" s="0" t="s">
+        <x:v>330</x:v>
+      </x:c>
+      <x:c r="E68" s="0" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="F68" s="0">
+        <x:v>992603</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:6">
+      <x:c r="A69" s="0">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>268</x:v>
+      </x:c>
+      <x:c r="C69" s="0">
+        <x:v>12340</x:v>
+      </x:c>
+      <x:c r="D69" s="0" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="E69" s="0" t="s">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="F69" s="0">
+        <x:v>874636</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:6">
+      <x:c r="A70" s="0">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="C70" s="0">
+        <x:v>17870</x:v>
+      </x:c>
+      <x:c r="D70" s="0" t="s">
+        <x:v>358</x:v>
+      </x:c>
+      <x:c r="E70" s="0" t="s">
+        <x:v>359</x:v>
+      </x:c>
+      <x:c r="F70" s="0">
+        <x:v>856825</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:6">
+      <x:c r="A71" s="0">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="C71" s="0">
+        <x:v>13580</x:v>
+      </x:c>
+      <x:c r="D71" s="0" t="s">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="E71" s="0" t="s">
+        <x:v>361</x:v>
+      </x:c>
+      <x:c r="F71" s="0">
+        <x:v>841195</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:6">
+      <x:c r="A75" s="0">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>362</x:v>
+      </x:c>
+      <x:c r="C75" s="0">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="D75" s="0" t="s">
+        <x:v>363</x:v>
+      </x:c>
+      <x:c r="E75" s="0" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="F75" s="0">
+        <x:v>813930</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:6">
+      <x:c r="A76" s="0">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="C76" s="0">
+        <x:v>14900</x:v>
+      </x:c>
+      <x:c r="D76" s="0" t="s">
+        <x:v>365</x:v>
+      </x:c>
+      <x:c r="E76" s="0" t="s">
+        <x:v>366</x:v>
+      </x:c>
+      <x:c r="F76" s="0">
+        <x:v>803088</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:6">
+      <x:c r="A77" s="0">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="C77" s="0">
+        <x:v>10980</x:v>
+      </x:c>
+      <x:c r="D77" s="0" t="s">
+        <x:v>367</x:v>
+      </x:c>
+      <x:c r="E77" s="0" t="s">
+        <x:v>368</x:v>
+      </x:c>
+      <x:c r="F77" s="0">
+        <x:v>786406</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:6">
+      <x:c r="A78" s="0">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="C78" s="0">
+        <x:v>2385</x:v>
+      </x:c>
+      <x:c r="D78" s="0" t="s">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="E78" s="0" t="s">
+        <x:v>369</x:v>
+      </x:c>
+      <x:c r="F78" s="0">
+        <x:v>763483</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:6">
+      <x:c r="A79" s="0">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C79" s="0">
+        <x:v>4720</x:v>
+      </x:c>
+      <x:c r="D79" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="E79" s="0" t="s">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="F79" s="0">
+        <x:v>719929</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:6">
+      <x:c r="A83" s="0">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="C83" s="0">
+        <x:v>12635</x:v>
+      </x:c>
+      <x:c r="D83" s="0" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="E83" s="0" t="s">
+        <x:v>371</x:v>
+      </x:c>
+      <x:c r="F83" s="0">
+        <x:v>662547</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:6">
+      <x:c r="A84" s="0">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>233</x:v>
+      </x:c>
+      <x:c r="C84" s="0">
+        <x:v>7445</x:v>
+      </x:c>
+      <x:c r="D84" s="0" t="s">
+        <x:v>372</x:v>
+      </x:c>
+      <x:c r="E84" s="0" t="s">
+        <x:v>373</x:v>
+      </x:c>
+      <x:c r="F84" s="0">
+        <x:v>648600</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:6">
+      <x:c r="A85" s="0">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="C85" s="0">
+        <x:v>42850</x:v>
+      </x:c>
+      <x:c r="D85" s="0" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="E85" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="F85" s="0">
+        <x:v>601475</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:6">
+      <x:c r="A86" s="0">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>374</x:v>
+      </x:c>
+      <x:c r="C86" s="0">
+        <x:v>9860</x:v>
+      </x:c>
+      <x:c r="D86" s="0" t="s">
+        <x:v>375</x:v>
+      </x:c>
+      <x:c r="E86" s="0" t="s">
+        <x:v>376</x:v>
+      </x:c>
+      <x:c r="F86" s="0">
+        <x:v>595904</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:6">
+      <x:c r="A87" s="0">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="C87" s="0">
+        <x:v>8210</x:v>
+      </x:c>
+      <x:c r="D87" s="0" t="s">
+        <x:v>377</x:v>
+      </x:c>
+      <x:c r="E87" s="0" t="s">
+        <x:v>378</x:v>
+      </x:c>
+      <x:c r="F87" s="0">
+        <x:v>593091</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:6">
+      <x:c r="A91" s="0">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="C91" s="0">
+        <x:v>71300</x:v>
+      </x:c>
+      <x:c r="D91" s="0" t="s">
+        <x:v>379</x:v>
+      </x:c>
+      <x:c r="E91" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="F91" s="0">
+        <x:v>588631</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:6">
+      <x:c r="A92" s="0">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="C92" s="0">
+        <x:v>8600</x:v>
+      </x:c>
+      <x:c r="D92" s="0" t="s">
+        <x:v>380</x:v>
+      </x:c>
+      <x:c r="E92" s="0" t="s">
+        <x:v>381</x:v>
+      </x:c>
+      <x:c r="F92" s="0">
+        <x:v>566213</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:6">
+      <x:c r="A93" s="0">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>382</x:v>
+      </x:c>
+      <x:c r="C93" s="0">
+        <x:v>9515</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="E93" s="0" t="s">
+        <x:v>383</x:v>
+      </x:c>
+      <x:c r="F93" s="0">
+        <x:v>556484</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:6">
+      <x:c r="A94" s="0">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="C94" s="0">
+        <x:v>34500</x:v>
+      </x:c>
+      <x:c r="D94" s="0" t="s">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="E94" s="0" t="s">
+        <x:v>385</x:v>
+      </x:c>
+      <x:c r="F94" s="0">
+        <x:v>552815</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:6">
+      <x:c r="A95" s="0">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>194</x:v>
+      </x:c>
+      <x:c r="C95" s="0">
+        <x:v>16860</x:v>
+      </x:c>
+      <x:c r="D95" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="E95" s="0" t="s">
+        <x:v>386</x:v>
+      </x:c>
+      <x:c r="F95" s="0">
+        <x:v>550840</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:6">
+      <x:c r="A99" s="0">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>387</x:v>
+      </x:c>
+      <x:c r="C99" s="0">
+        <x:v>22150</x:v>
+      </x:c>
+      <x:c r="D99" s="0" t="s">
+        <x:v>388</x:v>
+      </x:c>
+      <x:c r="E99" s="0" t="s">
+        <x:v>389</x:v>
+      </x:c>
+      <x:c r="F99" s="0">
+        <x:v>550303</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:6">
+      <x:c r="A100" s="0">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>390</x:v>
+      </x:c>
+      <x:c r="C100" s="0">
+        <x:v>5200</x:v>
+      </x:c>
+      <x:c r="D100" s="0" t="s">
+        <x:v>391</x:v>
+      </x:c>
+      <x:c r="E100" s="0" t="s">
+        <x:v>392</x:v>
+      </x:c>
+      <x:c r="F100" s="0">
+        <x:v>548508</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:6">
+      <x:c r="A101" s="0">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C101" s="0">
+        <x:v>5655</x:v>
+      </x:c>
+      <x:c r="D101" s="0" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="E101" s="0" t="s">
+        <x:v>393</x:v>
+      </x:c>
+      <x:c r="F101" s="0">
+        <x:v>532969</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:6">
+      <x:c r="A102" s="0">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
+        <x:v>394</x:v>
+      </x:c>
+      <x:c r="C102" s="0">
+        <x:v>10345</x:v>
+      </x:c>
+      <x:c r="D102" s="0" t="s">
+        <x:v>395</x:v>
+      </x:c>
+      <x:c r="E102" s="0" t="s">
+        <x:v>396</x:v>
+      </x:c>
+      <x:c r="F102" s="0">
+        <x:v>509017</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" spans="1:6">
+      <x:c r="A103" s="0">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B103" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="C103" s="0">
+        <x:v>18915</x:v>
+      </x:c>
+      <x:c r="D103" s="0" t="s">
+        <x:v>397</x:v>
+      </x:c>
+      <x:c r="E103" s="0" t="s">
+        <x:v>398</x:v>
+      </x:c>
+      <x:c r="F103" s="0">
+        <x:v>508089</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" spans="1:6">
+      <x:c r="A107" s="0">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B107" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+      <x:c r="C107" s="0">
+        <x:v>8685</x:v>
+      </x:c>
+      <x:c r="D107" s="0" t="s">
+        <x:v>379</x:v>
+      </x:c>
+      <x:c r="E107" s="0" t="s">
+        <x:v>399</x:v>
+      </x:c>
+      <x:c r="F107" s="0">
+        <x:v>507171</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" spans="1:6">
+      <x:c r="A108" s="0">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B108" s="0" t="s">
+        <x:v>400</x:v>
+      </x:c>
+      <x:c r="C108" s="0">
+        <x:v>846</x:v>
+      </x:c>
+      <x:c r="D108" s="0" t="s">
+        <x:v>401</x:v>
+      </x:c>
+      <x:c r="E108" s="0" t="s">
+        <x:v>402</x:v>
+      </x:c>
+      <x:c r="F108" s="0">
+        <x:v>464472</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" spans="1:6">
+      <x:c r="A109" s="0">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B109" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="C109" s="0">
+        <x:v>20400</x:v>
+      </x:c>
+      <x:c r="D109" s="0" t="s">
+        <x:v>403</x:v>
+      </x:c>
+      <x:c r="E109" s="0" t="s">
+        <x:v>404</x:v>
+      </x:c>
+      <x:c r="F109" s="0">
+        <x:v>464288</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110" spans="1:6">
+      <x:c r="A110" s="0">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B110" s="0" t="s">
+        <x:v>405</x:v>
+      </x:c>
+      <x:c r="C110" s="0">
+        <x:v>4320</x:v>
+      </x:c>
+      <x:c r="D110" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="E110" s="0" t="s">
+        <x:v>406</x:v>
+      </x:c>
+      <x:c r="F110" s="0">
+        <x:v>461010</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:6">
+      <x:c r="A111" s="0">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B111" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="C111" s="0">
+        <x:v>923</x:v>
+      </x:c>
+      <x:c r="D111" s="0" t="s">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="E111" s="0" t="s">
+        <x:v>407</x:v>
+      </x:c>
+      <x:c r="F111" s="0">
+        <x:v>452717</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="115" spans="1:6">
+      <x:c r="A115" s="0">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B115" s="0" t="s">
+        <x:v>408</x:v>
+      </x:c>
+      <x:c r="C115" s="0">
+        <x:v>7415</x:v>
+      </x:c>
+      <x:c r="D115" s="0" t="s">
+        <x:v>409</x:v>
+      </x:c>
+      <x:c r="E115" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="F115" s="0">
+        <x:v>444559</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116" spans="1:6">
+      <x:c r="A116" s="0">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B116" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="C116" s="0">
+        <x:v>9305</x:v>
+      </x:c>
+      <x:c r="D116" s="0" t="s">
+        <x:v>410</x:v>
+      </x:c>
+      <x:c r="E116" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="F116" s="0">
+        <x:v>435901</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="117" spans="1:6">
+      <x:c r="A117" s="0">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B117" s="0" t="s">
+        <x:v>411</x:v>
+      </x:c>
+      <x:c r="C117" s="0">
+        <x:v>14460</x:v>
+      </x:c>
+      <x:c r="D117" s="0" t="s">
+        <x:v>412</x:v>
+      </x:c>
+      <x:c r="E117" s="0" t="s">
+        <x:v>413</x:v>
+      </x:c>
+      <x:c r="F117" s="0">
+        <x:v>424347</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="118" spans="1:6">
+      <x:c r="A118" s="0">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B118" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="C118" s="0">
+        <x:v>8515</x:v>
+      </x:c>
+      <x:c r="D118" s="0" t="s">
+        <x:v>414</x:v>
+      </x:c>
+      <x:c r="E118" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="F118" s="0">
+        <x:v>400829</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="119" spans="1:6">
+      <x:c r="A119" s="0">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="B119" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="C119" s="0">
+        <x:v>9400</x:v>
+      </x:c>
+      <x:c r="D119" s="0" t="s">
+        <x:v>380</x:v>
+      </x:c>
+      <x:c r="E119" s="0" t="s">
+        <x:v>398</x:v>
+      </x:c>
+      <x:c r="F119" s="0">
+        <x:v>400608</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="123" spans="1:6">
+      <x:c r="A123" s="0">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B123" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="C123" s="0">
+        <x:v>20420</x:v>
+      </x:c>
+      <x:c r="D123" s="0" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="E123" s="0" t="s">
+        <x:v>415</x:v>
+      </x:c>
+      <x:c r="F123" s="0">
+        <x:v>392322</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="124" spans="1:6">
+      <x:c r="A124" s="0">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="B124" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+      <x:c r="C124" s="0">
+        <x:v>16860</x:v>
+      </x:c>
+      <x:c r="D124" s="0" t="s">
+        <x:v>417</x:v>
+      </x:c>
+      <x:c r="E124" s="0" t="s">
+        <x:v>418</x:v>
+      </x:c>
+      <x:c r="F124" s="0">
+        <x:v>388893</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="125" spans="1:6">
+      <x:c r="A125" s="0">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B125" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="C125" s="0">
+        <x:v>19550</x:v>
+      </x:c>
+      <x:c r="D125" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+      <x:c r="E125" s="0" t="s">
+        <x:v>420</x:v>
+      </x:c>
+      <x:c r="F125" s="0">
+        <x:v>386861</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="126" spans="1:6">
+      <x:c r="A126" s="0">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="B126" s="0" t="s">
+        <x:v>421</x:v>
+      </x:c>
+      <x:c r="C126" s="0">
+        <x:v>32595</x:v>
+      </x:c>
+      <x:c r="D126" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="E126" s="0" t="s">
+        <x:v>422</x:v>
+      </x:c>
+      <x:c r="F126" s="0">
+        <x:v>384313</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="127" spans="1:6">
+      <x:c r="A127" s="0">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B127" s="0" t="s">
+        <x:v>423</x:v>
+      </x:c>
+      <x:c r="C127" s="0">
+        <x:v>20450</x:v>
+      </x:c>
+      <x:c r="D127" s="0" t="s">
+        <x:v>424</x:v>
+      </x:c>
+      <x:c r="E127" s="0" t="s">
+        <x:v>425</x:v>
+      </x:c>
+      <x:c r="F127" s="0">
+        <x:v>379291</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="131" spans="1:6">
+      <x:c r="A131" s="0">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="B131" s="0" t="s">
+        <x:v>426</x:v>
+      </x:c>
+      <x:c r="C131" s="0">
+        <x:v>553</x:v>
+      </x:c>
+      <x:c r="D131" s="0" t="s">
+        <x:v>427</x:v>
+      </x:c>
+      <x:c r="E131" s="0" t="s">
+        <x:v>428</x:v>
+      </x:c>
+      <x:c r="F131" s="0">
+        <x:v>370673</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="132" spans="1:6">
+      <x:c r="A132" s="0">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B132" s="0" t="s">
+        <x:v>429</x:v>
+      </x:c>
+      <x:c r="C132" s="0">
+        <x:v>3680</x:v>
+      </x:c>
+      <x:c r="D132" s="0" t="s">
+        <x:v>430</x:v>
+      </x:c>
+      <x:c r="E132" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+      <x:c r="F132" s="0">
+        <x:v>369024</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="133" spans="1:6">
+      <x:c r="A133" s="0">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="B133" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="C133" s="0">
+        <x:v>7915</x:v>
+      </x:c>
+      <x:c r="D133" s="0" t="s">
+        <x:v>431</x:v>
+      </x:c>
+      <x:c r="E133" s="0" t="s">
+        <x:v>432</x:v>
+      </x:c>
+      <x:c r="F133" s="0">
+        <x:v>367748</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="134" spans="1:6">
+      <x:c r="A134" s="0">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B134" s="0" t="s">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="C134" s="0">
+        <x:v>1540</x:v>
+      </x:c>
+      <x:c r="D134" s="0" t="s">
+        <x:v>303</x:v>
+      </x:c>
+      <x:c r="E134" s="0" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="F134" s="0">
+        <x:v>362623</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="135" spans="1:6">
+      <x:c r="A135" s="0">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B135" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="C135" s="0">
+        <x:v>16570</x:v>
+      </x:c>
+      <x:c r="D135" s="0" t="s">
+        <x:v>330</x:v>
+      </x:c>
+      <x:c r="E135" s="0" t="s">
+        <x:v>378</x:v>
+      </x:c>
+      <x:c r="F135" s="0">
+        <x:v>355896</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139" spans="1:6">
+      <x:c r="A139" s="0">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B139" s="0" t="s">
+        <x:v>273</x:v>
+      </x:c>
+      <x:c r="C139" s="0">
+        <x:v>12350</x:v>
+      </x:c>
+      <x:c r="D139" s="0" t="s">
+        <x:v>434</x:v>
+      </x:c>
+      <x:c r="E139" s="0" t="s">
+        <x:v>435</x:v>
+      </x:c>
+      <x:c r="F139" s="0">
+        <x:v>353644</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140" spans="1:6">
+      <x:c r="A140" s="0">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="B140" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="C140" s="0">
+        <x:v>7365</x:v>
+      </x:c>
+      <x:c r="D140" s="0" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="E140" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F140" s="0">
+        <x:v>351805</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="141" spans="1:6">
+      <x:c r="A141" s="0">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B141" s="0" t="s">
+        <x:v>436</x:v>
+      </x:c>
+      <x:c r="C141" s="0">
+        <x:v>10615</x:v>
+      </x:c>
+      <x:c r="D141" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E141" s="0" t="s">
+        <x:v>437</x:v>
+      </x:c>
+      <x:c r="F141" s="0">
+        <x:v>351677</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="142" spans="1:6">
+      <x:c r="A142" s="0">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B142" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="C142" s="0">
+        <x:v>20060</x:v>
+      </x:c>
+      <x:c r="D142" s="0" t="s">
+        <x:v>438</x:v>
+      </x:c>
+      <x:c r="E142" s="0" t="s">
+        <x:v>439</x:v>
+      </x:c>
+      <x:c r="F142" s="0">
+        <x:v>342408</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="143" spans="1:6">
+      <x:c r="A143" s="0">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B143" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="C143" s="0">
+        <x:v>2690</x:v>
+      </x:c>
+      <x:c r="D143" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="E143" s="0" t="s">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="F143" s="0">
+        <x:v>341349</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="147" spans="1:6">
+      <x:c r="A147" s="0">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="B147" s="0" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="C147" s="0">
+        <x:v>4165</x:v>
+      </x:c>
+      <x:c r="D147" s="0" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="E147" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="F147" s="0">
+        <x:v>332770</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="148" spans="1:6">
+      <x:c r="A148" s="0">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B148" s="0" t="s">
+        <x:v>441</x:v>
+      </x:c>
+      <x:c r="C148" s="0">
+        <x:v>9380</x:v>
+      </x:c>
+      <x:c r="D148" s="0" t="s">
+        <x:v>395</x:v>
+      </x:c>
+      <x:c r="E148" s="0" t="s">
+        <x:v>442</x:v>
+      </x:c>
+      <x:c r="F148" s="0">
+        <x:v>332100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="149" spans="1:6">
+      <x:c r="A149" s="0">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B149" s="0" t="s">
+        <x:v>244</x:v>
+      </x:c>
+      <x:c r="C149" s="0">
+        <x:v>1402</x:v>
+      </x:c>
+      <x:c r="D149" s="0" t="s">
+        <x:v>443</x:v>
+      </x:c>
+      <x:c r="E149" s="0" t="s">
+        <x:v>193</x:v>
+      </x:c>
+      <x:c r="F149" s="0">
+        <x:v>328299</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="150" spans="1:6">
+      <x:c r="A150" s="0">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B150" s="0" t="s">
+        <x:v>247</x:v>
+      </x:c>
+      <x:c r="C150" s="0">
+        <x:v>9900</x:v>
+      </x:c>
+      <x:c r="D150" s="0" t="s">
+        <x:v>187</x:v>
+      </x:c>
+      <x:c r="E150" s="0" t="s">
+        <x:v>444</x:v>
+      </x:c>
+      <x:c r="F150" s="0">
+        <x:v>323968</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="151" spans="1:6">
+      <x:c r="A151" s="0">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B151" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="C151" s="0">
+        <x:v>46800</x:v>
+      </x:c>
+      <x:c r="D151" s="0" t="s">
+        <x:v>445</x:v>
+      </x:c>
+      <x:c r="E151" s="0" t="s">
+        <x:v>331</x:v>
+      </x:c>
+      <x:c r="F151" s="0">
+        <x:v>320394</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="155" spans="1:6">
+      <x:c r="A155" s="0">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B155" s="0" t="s">
+        <x:v>446</x:v>
+      </x:c>
+      <x:c r="C155" s="0">
+        <x:v>15010</x:v>
+      </x:c>
+      <x:c r="D155" s="0" t="s">
+        <x:v>377</x:v>
+      </x:c>
+      <x:c r="E155" s="0" t="s">
+        <x:v>447</x:v>
+      </x:c>
+      <x:c r="F155" s="0">
+        <x:v>319092</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="156" spans="1:6">
+      <x:c r="A156" s="0">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="B156" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="C156" s="0">
+        <x:v>6785</x:v>
+      </x:c>
+      <x:c r="D156" s="0" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="E156" s="0" t="s">
+        <x:v>449</x:v>
+      </x:c>
+      <x:c r="F156" s="0">
+        <x:v>313620</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="157" spans="1:6">
+      <x:c r="A157" s="0">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B157" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="C157" s="0">
+        <x:v>5040</x:v>
+      </x:c>
+      <x:c r="D157" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E157" s="0" t="s">
+        <x:v>450</x:v>
+      </x:c>
+      <x:c r="F157" s="0">
+        <x:v>305535</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="158" spans="1:6">
+      <x:c r="A158" s="0">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="B158" s="0" t="s">
+        <x:v>451</x:v>
+      </x:c>
+      <x:c r="C158" s="0">
+        <x:v>4680</x:v>
+      </x:c>
+      <x:c r="D158" s="0" t="s">
+        <x:v>312</x:v>
+      </x:c>
+      <x:c r="E158" s="0" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="F158" s="0">
+        <x:v>301057</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="159" spans="1:6">
+      <x:c r="A159" s="0">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B159" s="0" t="s">
+        <x:v>453</x:v>
+      </x:c>
+      <x:c r="C159" s="0">
+        <x:v>9115</x:v>
+      </x:c>
+      <x:c r="D159" s="0" t="s">
+        <x:v>318</x:v>
+      </x:c>
+      <x:c r="E159" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="F159" s="0">
+        <x:v>300691</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>